<commit_message>
Added a missing interval in Excel color test files
</commit_message>
<xml_diff>
--- a/src/test/resources/valid/color/allGreenTimeSlotsSchedule.xlsx
+++ b/src/test/resources/valid/color/allGreenTimeSlotsSchedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrutodea/dev/schedule-matcher/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrutodea/dev/schedule-matcher/src/test/resources/valid/color/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0884474A-186A-2B45-B13A-B263A73BB8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C817D322-D008-CB4B-8392-71D816C62A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{908E9387-ABF5-9B43-AAD6-F9C58C7F893A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Monday</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>16:00 - 17:00</t>
+  </si>
+  <si>
+    <t>9:00 - 10:00</t>
   </si>
 </sst>
 </file>
@@ -449,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5DE7AB4-C00E-AF44-A2EC-23C788DC93FF}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,7 +500,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -509,7 +512,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -521,7 +524,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -533,7 +536,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -545,7 +548,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -557,7 +560,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -569,7 +572,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -581,7 +584,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -593,7 +596,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -603,6 +606,18 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>